<commit_message>
cleaning up a bit
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11205"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5d13c61c60eae0c/Documents/College/IEEE/SplitKeyboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{5F774F9A-CF91-43CF-97CD-291A2CED57C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{136C86F2-FE3A-4250-93AE-F2EE3AF40FE6}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{5F774F9A-CF91-43CF-97CD-291A2CED57C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D559AD23-C38C-E84A-8F1B-C54B01A2C2B8}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15370" xr2:uid="{BF71731F-2AF2-4F8C-956A-20C0577DED67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -682,22 +682,22 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8671875" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="17.08203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" customWidth="1"/>
+    <col min="5" max="5" width="13.31640625" customWidth="1"/>
+    <col min="6" max="6" width="17.3515625" customWidth="1"/>
+    <col min="7" max="7" width="15.6015625" customWidth="1"/>
+    <col min="8" max="8" width="14.390625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:9" ht="29.25" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -736,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -753,7 +753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -782,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -799,7 +799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -816,7 +816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -839,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -856,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -879,7 +879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -905,7 +905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -925,7 +925,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -942,7 +942,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -956,7 +956,7 @@
         <v>42.99</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -964,7 +964,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
@@ -974,12 +974,12 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>81.64</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>66</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -999,12 +999,12 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>20.11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>63</v>
       </c>
@@ -1015,7 +1015,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>64</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>65</v>
       </c>

</xml_diff>